<commit_message>
Added Tests. Added Number String Format Modes and Negative Value Display Modes.
</commit_message>
<xml_diff>
--- a/notes/Notes02.xlsx
+++ b/notes/Notes02.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D38C340-9823-4051-AE66-C2C188AF3AE6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C5896A-EFC9-480F-A86A-423593FAECC4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Subtraction" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,8 @@
     <sheet name="Magnitude" sheetId="3" r:id="rId3"/>
     <sheet name="Division" sheetId="4" r:id="rId4"/>
     <sheet name="ArrayLengths" sheetId="5" r:id="rId5"/>
-    <sheet name="SquareRoot" sheetId="6" r:id="rId6"/>
+    <sheet name="Thousands" sheetId="7" r:id="rId6"/>
+    <sheet name="SquareRoot" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="61">
   <si>
     <t>N1</t>
   </si>
@@ -184,15 +185,46 @@
   </si>
   <si>
     <t>Integer Length - Precsion     =  16 - 9  = 7</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>Precision = 2</t>
+  </si>
+  <si>
+    <t>Length = 13</t>
+  </si>
+  <si>
+    <t>Absolute Number String</t>
+  </si>
+  <si>
+    <t>Comma Delimited Number String</t>
+  </si>
+  <si>
+    <t>Length = 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -234,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -263,6 +295,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2003,10 +2042,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D9B53F5-0109-45ED-9FFA-6981DEB334C5}">
-  <dimension ref="C3:Y28"/>
+  <dimension ref="C3:Y32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2489,6 +2528,47 @@
         <v>9</v>
       </c>
     </row>
+    <row r="32" spans="3:18" x14ac:dyDescent="0.25">
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>1</v>
+      </c>
+      <c r="G32" s="4">
+        <v>2</v>
+      </c>
+      <c r="H32" s="4">
+        <v>3</v>
+      </c>
+      <c r="I32" s="4">
+        <v>4</v>
+      </c>
+      <c r="J32" s="4">
+        <v>5</v>
+      </c>
+      <c r="K32" s="4">
+        <v>6</v>
+      </c>
+      <c r="L32" s="4">
+        <v>7</v>
+      </c>
+      <c r="M32" s="4">
+        <v>8</v>
+      </c>
+      <c r="N32" s="4">
+        <v>9</v>
+      </c>
+      <c r="O32" s="4">
+        <v>10</v>
+      </c>
+      <c r="P32" s="4">
+        <v>11</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E3:K3"/>
@@ -2500,6 +2580,253 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12545EB3-480A-45F5-AF36-3E98ACD91A97}">
+  <dimension ref="B2:S9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="19" width="5.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B2" s="14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B3" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12">
+        <v>0</v>
+      </c>
+      <c r="F3" s="12">
+        <f>1+E3</f>
+        <v>1</v>
+      </c>
+      <c r="G3" s="12">
+        <f>1+F3</f>
+        <v>2</v>
+      </c>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12">
+        <f>1+G3</f>
+        <v>3</v>
+      </c>
+      <c r="J3" s="12">
+        <f>1+I3</f>
+        <v>4</v>
+      </c>
+      <c r="K3" s="12">
+        <f>1+J3</f>
+        <v>5</v>
+      </c>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12">
+        <f>1+K3</f>
+        <v>6</v>
+      </c>
+      <c r="N3" s="12">
+        <f>1+M3</f>
+        <v>7</v>
+      </c>
+      <c r="O3" s="12">
+        <f t="shared" ref="O3:R3" si="0">1+N3</f>
+        <v>8</v>
+      </c>
+      <c r="P3" s="12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="Q3" s="12">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="R3" s="12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="S3" s="12"/>
+    </row>
+    <row r="4" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B4" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" s="13"/>
+      <c r="E4" s="12">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12">
+        <v>2</v>
+      </c>
+      <c r="G4" s="12">
+        <v>3</v>
+      </c>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12">
+        <v>4</v>
+      </c>
+      <c r="J4" s="12">
+        <v>5</v>
+      </c>
+      <c r="K4" s="12">
+        <v>6</v>
+      </c>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12">
+        <v>7</v>
+      </c>
+      <c r="N4" s="12">
+        <v>8</v>
+      </c>
+      <c r="O4" s="12">
+        <v>9</v>
+      </c>
+      <c r="P4" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="12">
+        <v>1</v>
+      </c>
+      <c r="R4" s="12">
+        <v>2</v>
+      </c>
+      <c r="S4" s="12"/>
+    </row>
+    <row r="7" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B7" s="14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="12">
+        <v>0</v>
+      </c>
+      <c r="E8" s="12">
+        <f>+D8+1</f>
+        <v>1</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" ref="F8:R8" si="1">+E8+1</f>
+        <v>2</v>
+      </c>
+      <c r="G8" s="12">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="H8" s="12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="J8" s="12">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="K8" s="12">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L8" s="12">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="M8" s="12">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="N8" s="12">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="O8" s="12">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="P8" s="12">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="Q8" s="12">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="R8" s="12">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="S8" s="12"/>
+    </row>
+    <row r="9" spans="2:19" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="B9" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="12">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>2</v>
+      </c>
+      <c r="G9" s="12">
+        <v>3</v>
+      </c>
+      <c r="H9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="I9" s="12">
+        <v>4</v>
+      </c>
+      <c r="J9" s="12">
+        <v>5</v>
+      </c>
+      <c r="K9" s="12">
+        <v>6</v>
+      </c>
+      <c r="L9" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="M9" s="12">
+        <v>7</v>
+      </c>
+      <c r="N9" s="12">
+        <v>8</v>
+      </c>
+      <c r="O9" s="12">
+        <v>9</v>
+      </c>
+      <c r="P9" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q9" s="12">
+        <v>1</v>
+      </c>
+      <c r="R9" s="12">
+        <v>2</v>
+      </c>
+      <c r="S9" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42BEE572-2FA7-4798-8197-A6A84AEE2BF8}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>